<commit_message>
IV regressions without murky cases
</commit_message>
<xml_diff>
--- a/Tables/iv_reg_def_notchoosing.xlsx
+++ b/Tables/iv_reg_def_notchoosing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533B979E-20DA-411C-B394-4C94B43B89E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8953D57E-265D-4D7B-B4F0-8C30710D68FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{8D8B75BE-A319-44D9-B827-2C4CDF107419}"/>
+    <workbookView xWindow="-28920" yWindow="-8820" windowWidth="29040" windowHeight="15720" xr2:uid="{8D8B75BE-A319-44D9-B827-2C4CDF107419}"/>
   </bookViews>
   <sheets>
     <sheet name="iv_reg_def_notchoosing" sheetId="1" r:id="rId1"/>
@@ -347,52 +347,52 @@
       <sheetData sheetId="0">
         <row r="5">
           <cell r="B5" t="str">
+            <v>0.021</v>
+          </cell>
+          <cell r="C5" t="str">
+            <v/>
+          </cell>
+          <cell r="D5" t="str">
+            <v/>
+          </cell>
+          <cell r="E5" t="str">
+            <v>-0.0087</v>
+          </cell>
+          <cell r="F5" t="str">
+            <v>-0.0015</v>
+          </cell>
+          <cell r="G5" t="str">
+            <v>0.011</v>
+          </cell>
+          <cell r="H5" t="str">
+            <v/>
+          </cell>
+          <cell r="I5" t="str">
+            <v/>
+          </cell>
+          <cell r="J5" t="str">
+            <v>-0.00037</v>
+          </cell>
+          <cell r="K5" t="str">
+            <v>-0.0024</v>
+          </cell>
+          <cell r="L5" t="str">
             <v>0.020</v>
           </cell>
-          <cell r="C5" t="str">
-            <v/>
-          </cell>
-          <cell r="D5" t="str">
-            <v/>
-          </cell>
-          <cell r="E5" t="str">
-            <v>-0.0089</v>
-          </cell>
-          <cell r="F5" t="str">
-            <v>-0.0019</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>0.0100</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v/>
-          </cell>
-          <cell r="I5" t="str">
-            <v/>
-          </cell>
-          <cell r="J5" t="str">
-            <v>-0.00064</v>
-          </cell>
-          <cell r="K5" t="str">
+          <cell r="M5" t="str">
+            <v/>
+          </cell>
+          <cell r="N5" t="str">
+            <v/>
+          </cell>
+          <cell r="O5" t="str">
+            <v>-0.0094</v>
+          </cell>
+          <cell r="P5" t="str">
             <v>-0.0027</v>
           </cell>
-          <cell r="L5" t="str">
-            <v>0.019</v>
-          </cell>
-          <cell r="M5" t="str">
-            <v/>
-          </cell>
-          <cell r="N5" t="str">
-            <v/>
-          </cell>
-          <cell r="O5" t="str">
-            <v>-0.0089</v>
-          </cell>
-          <cell r="P5" t="str">
-            <v>-0.0024</v>
-          </cell>
           <cell r="Q5" t="str">
-            <v>0.0093</v>
+            <v>0.0097</v>
           </cell>
           <cell r="R5" t="str">
             <v/>
@@ -401,7 +401,7 @@
             <v/>
           </cell>
           <cell r="T5" t="str">
-            <v>-0.0021</v>
+            <v>-0.0022</v>
           </cell>
           <cell r="U5" t="str">
             <v>-0.0041</v>
@@ -418,13 +418,13 @@
             <v/>
           </cell>
           <cell r="E6" t="str">
-            <v>(0.0032)</v>
+            <v>(0.0031)</v>
           </cell>
           <cell r="F6" t="str">
-            <v>(0.0032)</v>
+            <v>(0.0031)</v>
           </cell>
           <cell r="G6" t="str">
-            <v>(0.00084)</v>
+            <v>(0.00088)</v>
           </cell>
           <cell r="H6" t="str">
             <v/>
@@ -433,10 +433,10 @@
             <v/>
           </cell>
           <cell r="J6" t="str">
-            <v>(0.0047)</v>
+            <v>(0.0045)</v>
           </cell>
           <cell r="K6" t="str">
-            <v>(0.0047)</v>
+            <v>(0.0046)</v>
           </cell>
           <cell r="L6" t="str">
             <v>(0.00067)</v>
@@ -448,13 +448,13 @@
             <v/>
           </cell>
           <cell r="O6" t="str">
-            <v>(0.0034)</v>
+            <v>(0.0032)</v>
           </cell>
           <cell r="P6" t="str">
-            <v>(0.0034)</v>
+            <v>(0.0032)</v>
           </cell>
           <cell r="Q6" t="str">
-            <v>(0.00092)</v>
+            <v>(0.00095)</v>
           </cell>
           <cell r="R6" t="str">
             <v/>
@@ -463,10 +463,10 @@
             <v/>
           </cell>
           <cell r="T6" t="str">
-            <v>(0.0050)</v>
+            <v>(0.0049)</v>
           </cell>
           <cell r="U6" t="str">
-            <v>(0.0050)</v>
+            <v>(0.0049)</v>
           </cell>
         </row>
         <row r="8">
@@ -474,7 +474,7 @@
             <v/>
           </cell>
           <cell r="C8" t="str">
-            <v>-0.45</v>
+            <v>-0.42</v>
           </cell>
           <cell r="E8" t="str">
             <v/>
@@ -486,7 +486,7 @@
             <v/>
           </cell>
           <cell r="H8" t="str">
-            <v>-0.064</v>
+            <v>-0.035</v>
           </cell>
           <cell r="J8" t="str">
             <v/>
@@ -498,7 +498,7 @@
             <v/>
           </cell>
           <cell r="M8" t="str">
-            <v>-0.46</v>
+            <v>-0.47</v>
           </cell>
           <cell r="O8" t="str">
             <v/>
@@ -510,7 +510,7 @@
             <v/>
           </cell>
           <cell r="R8" t="str">
-            <v>-0.23</v>
+            <v>-0.22</v>
           </cell>
           <cell r="T8" t="str">
             <v/>
@@ -524,32 +524,32 @@
             <v/>
           </cell>
           <cell r="C9" t="str">
+            <v>(0.15)</v>
+          </cell>
+          <cell r="E9" t="str">
+            <v/>
+          </cell>
+          <cell r="F9" t="str">
+            <v/>
+          </cell>
+          <cell r="G9" t="str">
+            <v/>
+          </cell>
+          <cell r="H9" t="str">
+            <v>(0.43)</v>
+          </cell>
+          <cell r="J9" t="str">
+            <v/>
+          </cell>
+          <cell r="K9" t="str">
+            <v/>
+          </cell>
+          <cell r="L9" t="str">
+            <v/>
+          </cell>
+          <cell r="M9" t="str">
             <v>(0.16)</v>
           </cell>
-          <cell r="E9" t="str">
-            <v/>
-          </cell>
-          <cell r="F9" t="str">
-            <v/>
-          </cell>
-          <cell r="G9" t="str">
-            <v/>
-          </cell>
-          <cell r="H9" t="str">
-            <v>(0.47)</v>
-          </cell>
-          <cell r="J9" t="str">
-            <v/>
-          </cell>
-          <cell r="K9" t="str">
-            <v/>
-          </cell>
-          <cell r="L9" t="str">
-            <v/>
-          </cell>
-          <cell r="M9" t="str">
-            <v>(0.18)</v>
-          </cell>
           <cell r="O9" t="str">
             <v/>
           </cell>
@@ -560,7 +560,7 @@
             <v/>
           </cell>
           <cell r="R9" t="str">
-            <v>(0.54)</v>
+            <v>(0.51)</v>
           </cell>
           <cell r="T9" t="str">
             <v/>
@@ -574,7 +574,7 @@
             <v/>
           </cell>
           <cell r="C11" t="str">
-            <v>0.092</v>
+            <v>0.066</v>
           </cell>
           <cell r="D11" t="str">
             <v/>
@@ -589,7 +589,7 @@
             <v/>
           </cell>
           <cell r="H11" t="str">
-            <v>0.19</v>
+            <v>0.16</v>
           </cell>
           <cell r="I11" t="str">
             <v/>
@@ -604,7 +604,7 @@
             <v/>
           </cell>
           <cell r="M11" t="str">
-            <v>0.12</v>
+            <v>0.13</v>
           </cell>
           <cell r="N11" t="str">
             <v/>
@@ -639,38 +639,38 @@
             <v/>
           </cell>
           <cell r="C12" t="str">
+            <v>(0.15)</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v/>
+          </cell>
+          <cell r="E12" t="str">
+            <v/>
+          </cell>
+          <cell r="F12" t="str">
+            <v/>
+          </cell>
+          <cell r="G12" t="str">
+            <v/>
+          </cell>
+          <cell r="H12" t="str">
+            <v>(0.43)</v>
+          </cell>
+          <cell r="I12" t="str">
+            <v/>
+          </cell>
+          <cell r="J12" t="str">
+            <v/>
+          </cell>
+          <cell r="K12" t="str">
+            <v/>
+          </cell>
+          <cell r="L12" t="str">
+            <v/>
+          </cell>
+          <cell r="M12" t="str">
             <v>(0.16)</v>
           </cell>
-          <cell r="D12" t="str">
-            <v/>
-          </cell>
-          <cell r="E12" t="str">
-            <v/>
-          </cell>
-          <cell r="F12" t="str">
-            <v/>
-          </cell>
-          <cell r="G12" t="str">
-            <v/>
-          </cell>
-          <cell r="H12" t="str">
-            <v>(0.47)</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v/>
-          </cell>
-          <cell r="J12" t="str">
-            <v/>
-          </cell>
-          <cell r="K12" t="str">
-            <v/>
-          </cell>
-          <cell r="L12" t="str">
-            <v/>
-          </cell>
-          <cell r="M12" t="str">
-            <v>(0.18)</v>
-          </cell>
           <cell r="N12" t="str">
             <v/>
           </cell>
@@ -684,7 +684,7 @@
             <v/>
           </cell>
           <cell r="R12" t="str">
-            <v>(0.54)</v>
+            <v>(0.51)</v>
           </cell>
           <cell r="S12" t="str">
             <v/>
@@ -698,30 +698,30 @@
         </row>
         <row r="14">
           <cell r="D14" t="str">
-            <v>-0.099</v>
+            <v>-0.073</v>
           </cell>
           <cell r="I14" t="str">
-            <v>-0.27</v>
+            <v>-0.23</v>
           </cell>
           <cell r="N14" t="str">
-            <v>-0.13</v>
+            <v>-0.14</v>
           </cell>
           <cell r="S14" t="str">
-            <v>-0.44</v>
+            <v>-0.42</v>
           </cell>
         </row>
         <row r="15">
           <cell r="D15" t="str">
+            <v>(0.15)</v>
+          </cell>
+          <cell r="I15" t="str">
+            <v>(0.43)</v>
+          </cell>
+          <cell r="N15" t="str">
             <v>(0.16)</v>
           </cell>
-          <cell r="I15" t="str">
-            <v>(0.47)</v>
-          </cell>
-          <cell r="N15" t="str">
-            <v>(0.18)</v>
-          </cell>
           <cell r="S15" t="str">
-            <v>(0.54)</v>
+            <v>(0.51)</v>
           </cell>
         </row>
         <row r="21">
@@ -744,49 +744,49 @@
             <v>0.005</v>
           </cell>
           <cell r="G21" t="str">
-            <v>0.624</v>
+            <v>0.585</v>
           </cell>
           <cell r="H21" t="str">
-            <v>0.554</v>
+            <v>0.516</v>
           </cell>
           <cell r="I21" t="str">
-            <v>0.550</v>
+            <v>0.510</v>
           </cell>
           <cell r="J21" t="str">
-            <v>0.554</v>
+            <v>0.515</v>
           </cell>
           <cell r="K21" t="str">
-            <v>0.550</v>
+            <v>0.510</v>
           </cell>
           <cell r="L21" t="str">
             <v>0.013</v>
           </cell>
           <cell r="M21" t="str">
-            <v>0.013</v>
+            <v>0.012</v>
           </cell>
           <cell r="N21" t="str">
-            <v>0.006</v>
+            <v>0.005</v>
           </cell>
           <cell r="O21" t="str">
-            <v>0.006</v>
+            <v>0.005</v>
           </cell>
           <cell r="P21" t="str">
-            <v>0.006</v>
+            <v>0.005</v>
           </cell>
           <cell r="Q21" t="str">
-            <v>0.638</v>
+            <v>0.583</v>
           </cell>
           <cell r="R21" t="str">
-            <v>0.571</v>
+            <v>0.528</v>
           </cell>
           <cell r="S21" t="str">
-            <v>0.568</v>
+            <v>0.524</v>
           </cell>
           <cell r="T21" t="str">
-            <v>0.571</v>
+            <v>0.528</v>
           </cell>
           <cell r="U21" t="str">
-            <v>0.568</v>
+            <v>0.524</v>
           </cell>
         </row>
         <row r="22">
@@ -794,16 +794,16 @@
             <v>DepVarMean</v>
           </cell>
           <cell r="B22" t="str">
-            <v>0.012</v>
+            <v>0.013</v>
           </cell>
           <cell r="C22" t="str">
-            <v>0.74</v>
+            <v>0.73</v>
           </cell>
           <cell r="D22" t="str">
             <v>0.74</v>
           </cell>
           <cell r="E22" t="str">
-            <v>0.74</v>
+            <v>0.73</v>
           </cell>
           <cell r="F22" t="str">
             <v>0.74</v>
@@ -812,46 +812,46 @@
             <v>0.011</v>
           </cell>
           <cell r="H22" t="str">
-            <v>0.73</v>
+            <v>0.71</v>
           </cell>
           <cell r="I22" t="str">
-            <v>0.73</v>
+            <v>0.72</v>
           </cell>
           <cell r="J22" t="str">
-            <v>0.73</v>
+            <v>0.71</v>
           </cell>
           <cell r="K22" t="str">
-            <v>0.73</v>
+            <v>0.72</v>
           </cell>
           <cell r="L22" t="str">
             <v>0.012</v>
           </cell>
           <cell r="M22" t="str">
-            <v>0.75</v>
+            <v>0.74</v>
           </cell>
           <cell r="N22" t="str">
             <v>0.75</v>
           </cell>
           <cell r="O22" t="str">
-            <v>0.75</v>
+            <v>0.74</v>
           </cell>
           <cell r="P22" t="str">
             <v>0.75</v>
           </cell>
           <cell r="Q22" t="str">
-            <v>0.0097</v>
+            <v>0.0099</v>
           </cell>
           <cell r="R22" t="str">
-            <v>0.74</v>
+            <v>0.73</v>
           </cell>
           <cell r="S22" t="str">
-            <v>0.75</v>
+            <v>0.73</v>
           </cell>
           <cell r="T22" t="str">
-            <v>0.74</v>
+            <v>0.73</v>
           </cell>
           <cell r="U22" t="str">
-            <v>0.75</v>
+            <v>0.73</v>
           </cell>
         </row>
       </sheetData>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!B5</f>
-        <v>0.020</v>
+        <v>0.021</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C5</f>
@@ -1274,15 +1274,15 @@
       </c>
       <c r="E5" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!E5</f>
-        <v>-0.0089</v>
+        <v>-0.0087</v>
       </c>
       <c r="F5" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!F5</f>
-        <v>-0.0019</v>
+        <v>-0.0015</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!G5</f>
-        <v>0.0100</v>
+        <v>0.011</v>
       </c>
       <c r="H5" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H5</f>
@@ -1294,11 +1294,11 @@
       </c>
       <c r="J5" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J5</f>
-        <v>-0.00064</v>
+        <v>-0.00037</v>
       </c>
       <c r="K5" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!K5</f>
-        <v>-0.0027</v>
+        <v>-0.0024</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -1316,15 +1316,15 @@
       </c>
       <c r="E6" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!E6</f>
-        <v>(0.0032)</v>
+        <v>(0.0031)</v>
       </c>
       <c r="F6" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!F6</f>
-        <v>(0.0032)</v>
+        <v>(0.0031)</v>
       </c>
       <c r="G6" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!G6</f>
-        <v>(0.00084)</v>
+        <v>(0.00088)</v>
       </c>
       <c r="H6" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H6</f>
@@ -1336,11 +1336,11 @@
       </c>
       <c r="J6" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J6</f>
-        <v>(0.0047)</v>
+        <v>(0.0045)</v>
       </c>
       <c r="K6" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!K6</f>
-        <v>(0.0047)</v>
+        <v>(0.0046)</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -1353,11 +1353,11 @@
       </c>
       <c r="C7" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C8</f>
-        <v>-0.45</v>
+        <v>-0.42</v>
       </c>
       <c r="D7" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!D14</f>
-        <v>-0.099</v>
+        <v>-0.073</v>
       </c>
       <c r="E7" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!E8</f>
@@ -1373,11 +1373,11 @@
       </c>
       <c r="H7" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H8</f>
-        <v>-0.064</v>
+        <v>-0.035</v>
       </c>
       <c r="I7" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I14</f>
-        <v>-0.27</v>
+        <v>-0.23</v>
       </c>
       <c r="J7" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J8</f>
@@ -1395,11 +1395,11 @@
       </c>
       <c r="C8" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C9</f>
-        <v>(0.16)</v>
+        <v>(0.15)</v>
       </c>
       <c r="D8" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!D15</f>
-        <v>(0.16)</v>
+        <v>(0.15)</v>
       </c>
       <c r="E8" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!E9</f>
@@ -1415,11 +1415,11 @@
       </c>
       <c r="H8" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H9</f>
-        <v>(0.47)</v>
+        <v>(0.43)</v>
       </c>
       <c r="I8" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I15</f>
-        <v>(0.47)</v>
+        <v>(0.43)</v>
       </c>
       <c r="J8" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J9</f>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="C9" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C11</f>
-        <v>0.092</v>
+        <v>0.066</v>
       </c>
       <c r="D9" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!D11</f>
@@ -1460,7 +1460,7 @@
       </c>
       <c r="H9" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H11</f>
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="I9" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I11</f>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C12</f>
-        <v>(0.16)</v>
+        <v>(0.15)</v>
       </c>
       <c r="D10" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!D12</f>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="H10" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H12</f>
-        <v>(0.47)</v>
+        <v>(0.43)</v>
       </c>
       <c r="I10" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I12</f>
@@ -1583,23 +1583,23 @@
       </c>
       <c r="G12" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!G21</f>
-        <v>0.624</v>
+        <v>0.585</v>
       </c>
       <c r="H12" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H21</f>
-        <v>0.554</v>
+        <v>0.516</v>
       </c>
       <c r="I12" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I21</f>
-        <v>0.550</v>
+        <v>0.510</v>
       </c>
       <c r="J12" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J21</f>
-        <v>0.554</v>
+        <v>0.515</v>
       </c>
       <c r="K12" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!K21</f>
-        <v>0.550</v>
+        <v>0.510</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
@@ -1609,11 +1609,11 @@
       </c>
       <c r="B13" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!B22</f>
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="C13" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!C22</f>
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="D13" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!D22</f>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="E13" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!E22</f>
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="F13" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!F22</f>
@@ -1633,19 +1633,19 @@
       </c>
       <c r="H13" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!H22</f>
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="I13" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!I22</f>
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="J13" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!J22</f>
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="K13" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!K22</f>
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B22" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!L5</f>
-        <v>0.019</v>
+        <v>0.020</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M5</f>
@@ -1865,15 +1865,15 @@
       </c>
       <c r="E22" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O5</f>
-        <v>-0.0089</v>
+        <v>-0.0094</v>
       </c>
       <c r="F22" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!P5</f>
-        <v>-0.0024</v>
+        <v>-0.0027</v>
       </c>
       <c r="G22" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!Q5</f>
-        <v>0.0093</v>
+        <v>0.0097</v>
       </c>
       <c r="H22" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R5</f>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="J22" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T5</f>
-        <v>-0.0021</v>
+        <v>-0.0022</v>
       </c>
       <c r="K22" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!U5</f>
@@ -1907,15 +1907,15 @@
       </c>
       <c r="E23" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O6</f>
-        <v>(0.0034)</v>
+        <v>(0.0032)</v>
       </c>
       <c r="F23" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!P6</f>
-        <v>(0.0034)</v>
+        <v>(0.0032)</v>
       </c>
       <c r="G23" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!Q6</f>
-        <v>(0.00092)</v>
+        <v>(0.00095)</v>
       </c>
       <c r="H23" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R6</f>
@@ -1927,11 +1927,11 @@
       </c>
       <c r="J23" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T6</f>
-        <v>(0.0050)</v>
+        <v>(0.0049)</v>
       </c>
       <c r="K23" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!U6</f>
-        <v>(0.0050)</v>
+        <v>(0.0049)</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
@@ -1944,11 +1944,11 @@
       </c>
       <c r="C24" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M8</f>
-        <v>-0.46</v>
+        <v>-0.47</v>
       </c>
       <c r="D24" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N14</f>
-        <v>-0.13</v>
+        <v>-0.14</v>
       </c>
       <c r="E24" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O8</f>
@@ -1964,11 +1964,11 @@
       </c>
       <c r="H24" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R8</f>
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="I24" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!S14</f>
-        <v>-0.44</v>
+        <v>-0.42</v>
       </c>
       <c r="J24" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T8</f>
@@ -1986,11 +1986,11 @@
       </c>
       <c r="C25" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M9</f>
-        <v>(0.18)</v>
+        <v>(0.16)</v>
       </c>
       <c r="D25" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N15</f>
-        <v>(0.18)</v>
+        <v>(0.16)</v>
       </c>
       <c r="E25" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O9</f>
@@ -2006,11 +2006,11 @@
       </c>
       <c r="H25" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R9</f>
-        <v>(0.54)</v>
+        <v>(0.51)</v>
       </c>
       <c r="I25" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!S15</f>
-        <v>(0.54)</v>
+        <v>(0.51)</v>
       </c>
       <c r="J25" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T9</f>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="C26" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M11</f>
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="D26" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N11</f>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="C27" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M12</f>
-        <v>(0.18)</v>
+        <v>(0.16)</v>
       </c>
       <c r="D27" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N12</f>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="H27" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R12</f>
-        <v>(0.54)</v>
+        <v>(0.51)</v>
       </c>
       <c r="I27" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!S12</f>
@@ -2153,39 +2153,39 @@
       </c>
       <c r="C29" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M21</f>
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="D29" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N21</f>
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="E29" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O21</f>
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="F29" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!P21</f>
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="G29" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!Q21</f>
-        <v>0.638</v>
+        <v>0.583</v>
       </c>
       <c r="H29" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R21</f>
-        <v>0.571</v>
+        <v>0.528</v>
       </c>
       <c r="I29" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!S21</f>
-        <v>0.568</v>
+        <v>0.524</v>
       </c>
       <c r="J29" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T21</f>
-        <v>0.571</v>
+        <v>0.528</v>
       </c>
       <c r="K29" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!U21</f>
-        <v>0.568</v>
+        <v>0.524</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
@@ -2198,7 +2198,7 @@
       </c>
       <c r="C30" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!M22</f>
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="D30" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!N22</f>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="E30" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!O22</f>
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="F30" s="3" t="str">
         <f>[1]iv_reg_def_notchoosing!P22</f>
@@ -2214,23 +2214,23 @@
       </c>
       <c r="G30" s="4" t="str">
         <f>[1]iv_reg_def_notchoosing!Q22</f>
-        <v>0.0097</v>
+        <v>0.0099</v>
       </c>
       <c r="H30" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!R22</f>
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="I30" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!S22</f>
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
       <c r="J30" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!T22</f>
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="K30" s="16" t="str">
         <f>[1]iv_reg_def_notchoosing!U22</f>
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
@@ -2354,18 +2354,18 @@
     <row r="35" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>